<commit_message>
[FIX] Correção no tipo do TransactionItem utilizado nos TestCases
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\UiPath\ProjetoFinalDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A8032A-ECBF-4618-B669-189D1ECEFC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB285D4E-EE57-4A59-8DF2-2D36315BA2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1634,7 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>